<commit_message>
Add FromObjectName and ToObjectName
</commit_message>
<xml_diff>
--- a/mapping/mapSalesColumnNames.xlsx
+++ b/mapping/mapSalesColumnNames.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my_project\OpenLogic\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EADA81BA-A442-4BFF-9CBA-191D1551F4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D87566-C3EE-4421-BFE1-AF26BAA7DCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24180" yWindow="1080" windowWidth="17280" windowHeight="9960" xr2:uid="{BEC7F757-FF3E-4E21-A1C7-B71AFFB18E08}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{BEC7F757-FF3E-4E21-A1C7-B71AFFB18E08}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Time Period</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Constraint Set</t>
+  </si>
+  <si>
+    <t>VarType</t>
   </si>
 </sst>
 </file>
@@ -554,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3176383-67EB-4BBA-A9EC-44ACF360F726}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +779,9 @@
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>